<commit_message>
added updated schema and QuickDB text file to include local income tax data
</commit_message>
<xml_diff>
--- a/Resources/LocalIncTax.xlsx
+++ b/Resources/LocalIncTax.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michellechampagne/Desktop/BOOTCAMP/UPenn-Data---Project-3/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{73CF3E9F-B1DE-9141-95F6-7ECDC495AA98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F312E76C-7397-7244-B4A2-16F365043059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="660" windowWidth="33640" windowHeight="17440" activeTab="1" xr2:uid="{BF435ABC-EFF4-2640-95F6-88684172C25F}"/>
+    <workbookView xWindow="62540" yWindow="7620" windowWidth="33640" windowHeight="17440" activeTab="1" xr2:uid="{BF435ABC-EFF4-2640-95F6-88684172C25F}"/>
   </bookViews>
   <sheets>
     <sheet name="Local Income Tax" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4114" uniqueCount="1507">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4116" uniqueCount="1509">
   <si>
     <t>City</t>
   </si>
@@ -4580,6 +4580,12 @@
   </si>
   <si>
     <t>Null</t>
+  </si>
+  <si>
+    <t>https://smartasset.com/taxes/pennsylvania-tax-calculator?year=2019#us/income</t>
+  </si>
+  <si>
+    <t>Local Earned Income Tax</t>
   </si>
 </sst>
 </file>
@@ -4976,10 +4982,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{076F3C68-9017-0047-9BD0-10B7EC302C1C}">
-  <dimension ref="A1:H502"/>
+  <dimension ref="A1:K502"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4991,7 +4997,7 @@
     <col min="7" max="7" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5014,7 +5020,7 @@
         <v>1503</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -5037,8 +5043,11 @@
         <f t="array" ref="H2">_xlfn.XLOOKUP(G2,$A$2:$A$100,$B$2:$B$100,N/A,-1,)</f>
         <v>3.7499999999999999E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="K2" t="s">
+        <v>1508</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -5061,8 +5070,11 @@
         <f t="array" ref="H3">_xlfn.XLOOKUP(G3,$A$2:$A$100,$B$2:$B$100,N/A,-1,)</f>
         <v>#NAME?</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="K3" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -5086,7 +5098,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -5110,7 +5122,7 @@
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -5134,7 +5146,7 @@
         <v>3.7499999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -5158,7 +5170,7 @@
         <v>1.6500000000000001E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -5182,7 +5194,7 @@
         <v>1.975E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -5206,7 +5218,7 @@
         <v>1.6E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -5230,7 +5242,7 @@
         <v>1.6E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -5254,7 +5266,7 @@
         <v>1.6E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -5278,7 +5290,7 @@
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
@@ -5302,7 +5314,7 @@
         <v>2.2499999999999999E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
@@ -5326,7 +5338,7 @@
         <v>1.55E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
@@ -5350,7 +5362,7 @@
         <v>1.6E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
@@ -14623,8 +14635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09BEFC44-8BAE-E840-A68E-D8FA9232B557}">
   <dimension ref="A1:E502"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
-      <selection activeCell="C507" sqref="C507"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N141" sqref="N141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>